<commit_message>
ZSS-10 Freeze row causes chart disappear
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/issue3/book/10-chart.xlsx
+++ b/zss.test/src/main/webapp/issue3/book/10-chart.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="15" windowWidth="17055" windowHeight="9960"/>
+    <workbookView xWindow="480" yWindow="15" windowWidth="17055" windowHeight="9960" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet" sheetId="5" r:id="rId1"/>
+    <sheet name="Sheet0" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
   <si>
     <t>A</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -104,7 +106,7 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$B$5</c:f>
+              <c:f>Sheet!$B$2:$B$5</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -124,7 +126,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$5</c:f>
+              <c:f>Sheet!$C$2:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -149,7 +151,7 @@
           <c:order val="1"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$B$5</c:f>
+              <c:f>Sheet!$B$2:$B$5</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -169,7 +171,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$5</c:f>
+              <c:f>Sheet!$D$2:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -189,24 +191,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="55512448"/>
-        <c:axId val="105035648"/>
+        <c:axId val="73731456"/>
+        <c:axId val="60556416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="55512448"/>
+        <c:axId val="73731456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105035648"/>
+        <c:crossAx val="60556416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105035648"/>
+        <c:axId val="60556416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -214,7 +216,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55512448"/>
+        <c:crossAx val="73731456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -227,13 +229,156 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="zh-TW"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet0!$B$2:$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>D</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet0!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet0!$B$2:$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>D</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet0!$D$2:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="55838976"/>
+        <c:axId val="73232384"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="55838976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="73232384"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="73232384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="55838976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="zh-TW"/>
   <c:chart>
@@ -332,24 +477,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="63999360"/>
-        <c:axId val="111961216"/>
+        <c:axId val="73151616"/>
+        <c:axId val="73153152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="63999360"/>
+        <c:axId val="73151616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111961216"/>
+        <c:crossAx val="73153152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111961216"/>
+        <c:axId val="73153152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -357,26 +502,313 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63999360"/>
+        <c:crossAx val="73151616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="zh-TW"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>D</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>D</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="73173632"/>
+        <c:axId val="73191808"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="73173632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="73191808"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="73191808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="73173632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="Sunset.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1028700" y="3248025"/>
+          <a:ext cx="3505200" cy="2628900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="Sunset.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1028700" y="3248025"/>
+          <a:ext cx="3505200" cy="2628900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -804,7 +1236,130 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:D5"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O28" sqref="O28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="2" spans="2:4">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:D5"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R34" sqref="R34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="2" spans="2:4">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="5" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
@@ -864,7 +1419,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
@@ -877,7 +1432,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
ZSS-10, fix padding issue in client
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/issue3/book/10-chart.xlsx
+++ b/zss.test/src/main/webapp/issue3/book/10-chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="15" windowWidth="17055" windowHeight="9960" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="15" windowWidth="17055" windowHeight="9960" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="5" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
+    <sheet name="Deep" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
   <si>
     <t>A</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -33,6 +34,22 @@
   </si>
   <si>
     <t>D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scroll to row 500 or column GR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -191,24 +208,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="73731456"/>
-        <c:axId val="60556416"/>
+        <c:axId val="55769728"/>
+        <c:axId val="76509568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="73731456"/>
+        <c:axId val="55769728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60556416"/>
+        <c:crossAx val="76509568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60556416"/>
+        <c:axId val="76509568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -216,7 +233,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73731456"/>
+        <c:crossAx val="55769728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -229,7 +246,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -334,24 +351,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="55838976"/>
-        <c:axId val="73232384"/>
+        <c:axId val="76428800"/>
+        <c:axId val="76430336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="55838976"/>
+        <c:axId val="76428800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73232384"/>
+        <c:crossAx val="76430336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73232384"/>
+        <c:axId val="76430336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -359,7 +376,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55838976"/>
+        <c:crossAx val="76428800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -372,7 +389,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -477,24 +494,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="73151616"/>
-        <c:axId val="73153152"/>
+        <c:axId val="77033472"/>
+        <c:axId val="77035008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="73151616"/>
+        <c:axId val="77033472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73153152"/>
+        <c:crossAx val="77035008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73153152"/>
+        <c:axId val="77035008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -502,7 +519,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73151616"/>
+        <c:crossAx val="77033472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -514,7 +531,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -619,24 +636,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="73173632"/>
-        <c:axId val="73191808"/>
+        <c:axId val="77055488"/>
+        <c:axId val="77057024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="73173632"/>
+        <c:axId val="77055488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73191808"/>
+        <c:crossAx val="77057024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73191808"/>
+        <c:axId val="77057024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -644,7 +661,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73173632"/>
+        <c:crossAx val="77055488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -656,7 +673,174 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="zh-TW"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.5946631671041121E-2"/>
+          <c:y val="7.4548702245552642E-2"/>
+          <c:w val="0.73269356955380582"/>
+          <c:h val="0.79822506561679785"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Deep!$B$489:$B$491</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Deep!$C$489:$C$491</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="77898496"/>
+        <c:axId val="77900032"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="77898496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="77900032"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="77900032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="77898496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="zh-TW"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:explosion val="25"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Deep!$GI$1:$GI$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>E</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>F</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>G</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Deep!$GJ$1:$GJ$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -941,6 +1125,71 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>472</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>486</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>185</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>189</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1297,7 +1546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="R34" sqref="R34"/>
     </sheetView>
@@ -1443,4 +1692,75 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:GJ491"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="4" topLeftCell="GD5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="GI16" sqref="GI16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1" spans="4:192">
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="GI1" t="s">
+        <v>5</v>
+      </c>
+      <c r="GJ1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="4:192">
+      <c r="GI2" t="s">
+        <v>6</v>
+      </c>
+      <c r="GJ2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="4:192">
+      <c r="GI3" t="s">
+        <v>7</v>
+      </c>
+      <c r="GJ3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="489" spans="2:3">
+      <c r="B489" t="s">
+        <v>0</v>
+      </c>
+      <c r="C489">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="490" spans="2:3">
+      <c r="B490" t="s">
+        <v>1</v>
+      </c>
+      <c r="C490">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="491" spans="2:3">
+      <c r="B491" t="s">
+        <v>2</v>
+      </c>
+      <c r="C491">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update release for series fix of ZSS-10 , including,  ZSS-455, ZSS-312, ZSS-458, ZSS-311 When you move a chart, it should become selected.
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/issue3/book/10-chart.xlsx
+++ b/zss.test/src/main/webapp/issue3/book/10-chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="15" windowWidth="17055" windowHeight="9960" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="15" windowWidth="17055" windowHeight="9960" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="5" r:id="rId1"/>
@@ -208,24 +208,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="55769728"/>
-        <c:axId val="76509568"/>
+        <c:axId val="76510720"/>
+        <c:axId val="76512640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="55769728"/>
+        <c:axId val="76510720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76509568"/>
+        <c:crossAx val="76512640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76509568"/>
+        <c:axId val="76512640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -233,20 +233,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55769728"/>
+        <c:crossAx val="76510720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -351,24 +350,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="76428800"/>
-        <c:axId val="76430336"/>
+        <c:axId val="77904896"/>
+        <c:axId val="79961472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="76428800"/>
+        <c:axId val="77904896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76430336"/>
+        <c:crossAx val="79961472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76430336"/>
+        <c:axId val="79961472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -376,20 +375,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76428800"/>
+        <c:crossAx val="77904896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -494,24 +492,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="77033472"/>
-        <c:axId val="77035008"/>
+        <c:axId val="80015360"/>
+        <c:axId val="80017280"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="77033472"/>
+        <c:axId val="80015360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77035008"/>
+        <c:crossAx val="80017280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77035008"/>
+        <c:axId val="80017280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -519,19 +517,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77033472"/>
+        <c:crossAx val="80015360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -636,24 +635,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="77055488"/>
-        <c:axId val="77057024"/>
+        <c:axId val="55959552"/>
+        <c:axId val="55961088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="77055488"/>
+        <c:axId val="55959552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77057024"/>
+        <c:crossAx val="55961088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77057024"/>
+        <c:axId val="55961088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -661,19 +660,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77055488"/>
+        <c:crossAx val="55959552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -691,7 +691,7 @@
           <c:yMode val="edge"/>
           <c:x val="8.5946631671041121E-2"/>
           <c:y val="7.4548702245552642E-2"/>
-          <c:w val="0.73269356955380582"/>
+          <c:w val="0.73269356955380593"/>
           <c:h val="0.79822506561679785"/>
         </c:manualLayout>
       </c:layout>
@@ -737,24 +737,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="77898496"/>
-        <c:axId val="77900032"/>
+        <c:axId val="61233024"/>
+        <c:axId val="61234560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="77898496"/>
+        <c:axId val="61233024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77900032"/>
+        <c:crossAx val="61234560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77900032"/>
+        <c:axId val="61234560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -762,20 +762,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77898496"/>
+        <c:crossAx val="61233024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -840,7 +839,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1608,11 +1607,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="7" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="L23" sqref="L23"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1698,7 +1697,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:GJ491"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="4" topLeftCell="GD5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>

</xml_diff>